<commit_message>
Cambios en tabla servicios
Se agregaron nuevos campos en la tabla servicios para una mejor relación de las tablas
</commit_message>
<xml_diff>
--- a/tablasVat.xlsx
+++ b/tablasVat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SebastianM\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SebastianM\Desktop\vat\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="143">
   <si>
     <t>Equipo</t>
   </si>
@@ -279,9 +279,6 @@
     <t>Contenido de Operacion</t>
   </si>
   <si>
-    <t>VarChar()45</t>
-  </si>
-  <si>
     <t>MantenimientoEquipos</t>
   </si>
   <si>
@@ -454,6 +451,9 @@
   </si>
   <si>
     <t>Operativo</t>
+  </si>
+  <si>
+    <t>Servicioscol</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1204,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1212,7 +1212,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1342,7 +1342,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1394,7 +1394,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1437,7 +1437,7 @@
         <v>48</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
         <v>58</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
@@ -1508,7 +1508,7 @@
         <v>59</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1562,10 +1562,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88:A90"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,7 +1579,7 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="25"/>
       <c r="B1" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C1" s="25"/>
     </row>
@@ -1594,13 +1594,13 @@
         <v>70</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" t="s">
         <v>133</v>
-      </c>
-      <c r="H2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1614,13 +1614,13 @@
         <v>72</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" t="s">
         <v>135</v>
-      </c>
-      <c r="H3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1634,16 +1634,16 @@
         <v>73</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" t="s">
         <v>137</v>
       </c>
-      <c r="H4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>74</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1710,22 +1710,22 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
       <c r="B13" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="25"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>75</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1733,13 +1733,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1747,13 +1747,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>78</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1767,7 +1767,7 @@
         <v>76</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1837,11 +1837,11 @@
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
       <c r="B29" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="25"/>
     </row>
-    <row r="30" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>83</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>75</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1866,7 +1866,7 @@
         <v>72</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1877,10 +1877,10 @@
         <v>82</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1894,7 +1894,7 @@
         <v>76</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1911,22 +1911,22 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="25"/>
       <c r="B37" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" s="25"/>
     </row>
     <row r="38" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>75</v>
       </c>
       <c r="D38" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1934,13 +1934,13 @@
         <v>30</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1948,13 +1948,13 @@
         <v>32</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>78</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1965,7 +1965,7 @@
         <v>76</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1982,25 +1982,25 @@
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="25"/>
       <c r="B44" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C44" s="25"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>75</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2008,13 +2008,13 @@
         <v>34</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2022,13 +2022,13 @@
         <v>35</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>78</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
@@ -2042,7 +2042,7 @@
         <v>76</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2066,31 +2066,31 @@
       </c>
       <c r="C51" s="26"/>
       <c r="D51" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="17"/>
       <c r="B52" s="20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D52" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="16"/>
       <c r="B53" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2099,45 +2099,45 @@
         <v>41</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D54" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="16"/>
       <c r="B55" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>78</v>
       </c>
       <c r="D55" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="16"/>
       <c r="B56" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D57" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2161,97 +2161,97 @@
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="28"/>
       <c r="B61" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="16"/>
       <c r="B62" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="16"/>
       <c r="B63" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>78</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="16"/>
       <c r="B64" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="16"/>
       <c r="B65" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="16"/>
       <c r="B66" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="16"/>
       <c r="B67" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="16"/>
       <c r="B68" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2262,7 +2262,7 @@
         <v>72</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2273,7 +2273,7 @@
         <v>76</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2292,10 +2292,10 @@
         <v>11</v>
       </c>
       <c r="C72" s="29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2308,121 +2308,121 @@
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="28"/>
       <c r="B74" s="27" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C74" s="18" t="s">
         <v>75</v>
       </c>
       <c r="D74" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="16"/>
       <c r="B75" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="16"/>
       <c r="B76" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>78</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="16"/>
       <c r="B77" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="16"/>
       <c r="B78" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="16"/>
       <c r="B79" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="16"/>
       <c r="B80" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D80" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="16"/>
       <c r="B81" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>76</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="16"/>
       <c r="B82" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D82" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="16"/>
       <c r="B83" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>72</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2434,7 +2434,7 @@
         <v>76</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2448,53 +2448,86 @@
         <v>1</v>
       </c>
     </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="25"/>
-      <c r="B87" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="C87" s="25"/>
+      <c r="B87" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="14" t="s">
+      <c r="B88" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="25"/>
+      <c r="B90" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C90" s="25"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B91" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="C91" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D91" s="31" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B88" s="27" t="s">
+      <c r="B92" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B93" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C88" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D88" s="31" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C90" s="8" t="s">
+      <c r="C93" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D90" s="8" t="s">
-        <v>140</v>
+      <c r="D93" s="8" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>